<commit_message>
After cantSplit attribute append
</commit_message>
<xml_diff>
--- a/conf.xlsx
+++ b/conf.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="0" userName="dpaspa"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="1" xWindow="240" yWindow="60" windowWidth="25380" windowHeight="11235" tabRatio="500"/>
+    <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="25380" windowHeight="11235" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="shell" sheetId="1" r:id="rId4"/>
@@ -13,23 +13,24 @@
     <sheet name="revHistory" sheetId="3" r:id="rId6"/>
     <sheet name="dataConnections" sheetId="4" r:id="rId7"/>
     <sheet name="dataMarkers" sheetId="5" r:id="rId8"/>
-    <sheet name="docParent" sheetId="6" r:id="rId9"/>
-    <sheet name="docChild" sheetId="7" r:id="rId10"/>
+    <sheet name="timeMarkers" sheetId="6" r:id="rId9"/>
+    <sheet name="docParent" sheetId="7" r:id="rId10"/>
+    <sheet name="docChild" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1540016988" val="934" rev="123" rev64="64" revOS="3"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1540016988" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1540016988" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1540016988"/>
+      <pm:revision xmlns:pm="smNativeData" day="1540462101" val="934" rev="123" rev64="64" revOS="3"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1540462101" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1540462101" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1540462101"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="307">
   <si>
     <t>projectName</t>
   </si>
@@ -82,7 +83,7 @@
     <t>cipsip</t>
   </si>
   <si>
-    <t>python fdg.py -c ./conf.xlsx -o /home/dpaspa/Dropbox/Business/Synertec/MPI.SMS/automation/code/docs/report/data/output -i /home/dpaspa/Dropbox/Business/Synertec/MPI.SMS/automation/code/docs/report/data/hmiM1_180928144537 -n cipsip -r Y -f 37</t>
+    <t>python fdg.py -c ./conf.xlsx -o /home/dpaspa/Dropbox/Business/Synertec/MPI.SMS/automation/code/docs/report/data/output -i /home/dpaspa/Dropbox/Business/Synertec/MPI.SMS/automation/code/docs/report/data/hmiM1_180928144537 -n cipsip -r Y -f 50\</t>
   </si>
   <si>
     <t>docPrefix</t>
@@ -505,10 +506,10 @@
     <t>Physical Class Installation Test Sheet - Storage Vessel S2</t>
   </si>
   <si>
-    <t>A170810-SAT-M1-LC-001</t>
-  </si>
-  <si>
-    <t>Site Acceptance Test - Configuration Verification for Manufacturing Vessel M1</t>
+    <t>A170810-SAT-M1-IC-002</t>
+  </si>
+  <si>
+    <t>Site Acceptance Test - Configuration Test for Manufacturing Vessel M1</t>
   </si>
   <si>
     <t>LC</t>
@@ -517,25 +518,25 @@
     <t>Loopchecks</t>
   </si>
   <si>
-    <t>A170810-SAT-M2-LC-001</t>
-  </si>
-  <si>
-    <t>Site Acceptance Test - Configuration Verification for Manufacturing Vessel M2</t>
-  </si>
-  <si>
-    <t>A170810-SAT-S1-LC-001</t>
-  </si>
-  <si>
-    <t>Site Acceptance Test - Configuration Verification for Storage Vessel S1</t>
-  </si>
-  <si>
-    <t>A170810-SAT-S2-LC-001</t>
-  </si>
-  <si>
-    <t>Site Acceptance Test - Configuration Verification for Storage Vessel S2</t>
-  </si>
-  <si>
-    <t>A170810-SAT-M1-IL-001</t>
+    <t>A170810-SAT-M2-IC-002</t>
+  </si>
+  <si>
+    <t>Site Acceptance Test - Configuration Test for Manufacturing Vessel M2</t>
+  </si>
+  <si>
+    <t>A170810-SAT-S1-IC-002</t>
+  </si>
+  <si>
+    <t>Site Acceptance Test - Configuration Test for Storage Vessel S1</t>
+  </si>
+  <si>
+    <t>A170810-SAT-S2-IC-002</t>
+  </si>
+  <si>
+    <t>Site Acceptance Test - Configuration Test for Storage Vessel S2</t>
+  </si>
+  <si>
+    <t>A170810-SAT-M1-IC-003</t>
   </si>
   <si>
     <t>Site Acceptance Test - Interlocks for Manufacturing Vessel M1</t>
@@ -544,19 +545,19 @@
     <t>Interlocks</t>
   </si>
   <si>
-    <t>A170810-SAT-M2-IL-001</t>
+    <t>A170810-SAT-M2-IC-003</t>
   </si>
   <si>
     <t>Site Acceptance Test - Interlocks for Manufacturing Vessel M2</t>
   </si>
   <si>
-    <t>A170810-SAT-S1-IL-001</t>
+    <t>A170810-SAT-S1-IC-003</t>
   </si>
   <si>
     <t>Site Acceptance Test - Interlocks for Storage Vessel S1</t>
   </si>
   <si>
-    <t>A170810-SAT-S2-IL-001</t>
+    <t>A170810-SAT-S2-IC-003</t>
   </si>
   <si>
     <t>Site Acceptance Test - Interlocks for Storage Vessel S2</t>
@@ -637,6 +638,18 @@
     <t>Not in MPI</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>report</t>
+  </si>
+  <si>
+    <t>A170810-RPT-001</t>
+  </si>
+  <si>
+    <t>CIPSIP</t>
+  </si>
+  <si>
     <t>Ver</t>
   </si>
   <si>
@@ -760,120 +773,63 @@
     <t>fileInputData</t>
   </si>
   <si>
-    <t>dbOutputName</t>
-  </si>
-  <si>
     <t>/home/dpaspa/Dropbox/Business/Synertec/MPI.SMS/automation/code/config</t>
   </si>
   <si>
     <t>config.xlsx</t>
   </si>
   <si>
-    <t>config</t>
-  </si>
-  <si>
     <t>/home/dpaspa/MEGA/Business/Synertec/AIN/reloaded</t>
   </si>
   <si>
     <t>s.xlsx</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>logAlarmBlock0</t>
-  </si>
-  <si>
     <t>logAlarmBlock0.csv</t>
   </si>
   <si>
-    <t>logEventConfirm0</t>
-  </si>
-  <si>
     <t>logEventConfirm0.csv</t>
   </si>
   <si>
-    <t>logEventMsg0</t>
-  </si>
-  <si>
     <t>logEventMsg0.csv</t>
   </si>
   <si>
-    <t>logEventPrompt0</t>
-  </si>
-  <si>
     <t>logEventPrompt0.csv</t>
   </si>
   <si>
-    <t>logEventReal0</t>
-  </si>
-  <si>
     <t>logEventReal0.csv</t>
   </si>
   <si>
-    <t>logEventTime0</t>
-  </si>
-  <si>
     <t>logEventTime0.csv</t>
   </si>
   <si>
-    <t>logMIn1010</t>
-  </si>
-  <si>
     <t>logMIn1010.csv</t>
   </si>
   <si>
-    <t>logOperatorAction0</t>
-  </si>
-  <si>
     <t>logOperatorAction0.csv</t>
   </si>
   <si>
-    <t>logPIn1030</t>
-  </si>
-  <si>
     <t>logPIn1030.csv</t>
   </si>
   <si>
-    <t>logSICn1010</t>
-  </si>
-  <si>
     <t>logSICn1010.csv</t>
   </si>
   <si>
-    <t>logTIn1010</t>
-  </si>
-  <si>
     <t>logTIn1010.csv</t>
   </si>
   <si>
-    <t>logTIn1030</t>
-  </si>
-  <si>
     <t>logTIn1030.csv</t>
   </si>
   <si>
-    <t>logTIn1050</t>
-  </si>
-  <si>
     <t>logTIn1050.csv</t>
   </si>
   <si>
-    <t>logTIn1070</t>
-  </si>
-  <si>
     <t>logTIn1070.csv</t>
   </si>
   <si>
-    <t>logTIn1090</t>
-  </si>
-  <si>
     <t>logTIn1090.csv</t>
   </si>
   <si>
-    <t>logTIn1110</t>
-  </si>
-  <si>
     <t>logTIn1110.csv</t>
   </si>
   <si>
@@ -883,19 +839,22 @@
     <t>markerEventString</t>
   </si>
   <si>
-    <t>filterData</t>
-  </si>
-  <si>
-    <t>timeBegin</t>
-  </si>
-  <si>
-    <t>1082,"@@FILTER@@"</t>
-  </si>
-  <si>
-    <t>timeEnd</t>
-  </si>
-  <si>
-    <t>1083,"@@FILTER@@"</t>
+    <t>begin</t>
+  </si>
+  <si>
+    <t>1068,"@@FILTER@@"</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>909,"@@FILTER@@"</t>
+  </si>
+  <si>
+    <t>850,"@@FILTER@@"</t>
+  </si>
+  <si>
+    <t>571,"@@FILTER@@"</t>
   </si>
   <si>
     <t>fileInput</t>
@@ -919,6 +878,9 @@
     <t>/home/dpaspa/Dropbox/Business/Synertec/MPI.SMS/automation/code/docs/tstClassPhysicalInstall.docx</t>
   </si>
   <si>
+    <t>T</t>
+  </si>
+  <si>
     <t>/home/dpaspa/Dropbox/Business/Synertec/MPI.SMS/automation/code/docs/tstClassSoftwareAlarmParent.docx</t>
   </si>
   <si>
@@ -980,9 +942,6 @@
   </si>
   <si>
     <t>/home/dpaspa/Dropbox/Business/Synertec/MPI.SMS/automation/code/docs/tstClassSoftwareAlarmChild.docx</t>
-  </si>
-  <si>
-    <t>T</t>
   </si>
   <si>
     <t>dataSheetTest</t>
@@ -1017,7 +976,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1540016988" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1540462101" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1032,7 +991,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1540016988" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1540462101" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1048,7 +1007,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1540016988" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1540462101" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -1070,7 +1029,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1540016988" type="1" fgLvl="100" fgClr="00B7DEE8" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1540462101" type="1" fgLvl="100" fgClr="00B7DEE8" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1081,7 +1040,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1540016988" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1540462101" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1092,7 +1051,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1540016988" type="1" fgLvl="100" fgClr="008EA9DB" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1540462101" type="1" fgLvl="100" fgClr="008EA9DB" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1103,7 +1062,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1540016988" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1540462101" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1125,7 +1084,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1540016988"/>
+          <pm:border xmlns:pm="smNativeData" id="1540462101"/>
         </ext>
       </extLst>
     </border>
@@ -1144,7 +1103,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1540016988"/>
+          <pm:border xmlns:pm="smNativeData" id="1540462101"/>
         </ext>
       </extLst>
     </border>
@@ -1163,7 +1122,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1540016988"/>
+          <pm:border xmlns:pm="smNativeData" id="1540462101"/>
         </ext>
       </extLst>
     </border>
@@ -1182,7 +1141,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1540016988"/>
+          <pm:border xmlns:pm="smNativeData" id="1540462101"/>
         </ext>
       </extLst>
     </border>
@@ -1201,7 +1160,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1540016988"/>
+          <pm:border xmlns:pm="smNativeData" id="1540462101"/>
         </ext>
       </extLst>
     </border>
@@ -1233,10 +1192,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1540016988" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1540462101" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1540016988" count="2">
+      <pm:colors xmlns:pm="smNativeData" id="1540462101" count="2">
         <pm:color name="Color 24" rgb="B7DEE8"/>
         <pm:color name="Color 25" rgb="8EA9DB"/>
       </pm:colors>
@@ -1474,8 +1433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="15.40"/>
@@ -1560,7 +1519,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1540016988" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1540462101" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1569,14 +1528,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1540016988" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1540016988" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1540462101" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1540462101" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1540016988" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1540462101" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1587,11 +1546,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L62"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F48" sqref="F48"/>
+    <sheetView view="normal" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
@@ -2880,11 +2839,31 @@
       </c>
       <c r="J62" s="8"/>
     </row>
+    <row r="63" spans="2:7">
+      <c r="B63" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1540016988" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1540462101" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2893,14 +2872,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1540016988" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1540016988" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1540462101" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1540462101" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1540016988" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1540462101" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -2911,11 +2890,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
@@ -2941,42 +2920,42 @@
         <v>20</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E2" s="5" t="n">
         <v>43052</v>
@@ -2994,24 +2973,24 @@
         <v>2017</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E3" s="5" t="n">
         <v>43052</v>
@@ -3029,24 +3008,24 @@
         <v>2017</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E4" s="5" t="n">
         <v>43052</v>
@@ -3064,24 +3043,24 @@
         <v>2017</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E5" s="5" t="n">
         <v>43053</v>
@@ -3099,24 +3078,24 @@
         <v>2017</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E6" s="5" t="n">
         <v>43052</v>
@@ -3134,24 +3113,24 @@
         <v>2017</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E7" s="5" t="n">
         <v>43052</v>
@@ -3169,24 +3148,24 @@
         <v>2017</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E8" s="5" t="n">
         <v>43052</v>
@@ -3204,24 +3183,24 @@
         <v>2017</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E9" s="5" t="n">
         <v>43052</v>
@@ -3239,24 +3218,24 @@
         <v>2017</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E10" s="5" t="n">
         <v>43052</v>
@@ -3274,24 +3253,24 @@
         <v>2017</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E11" s="5" t="n">
         <v>43052</v>
@@ -3309,24 +3288,24 @@
         <v>2017</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E12" s="5" t="n">
         <v>43052</v>
@@ -3344,24 +3323,24 @@
         <v>2017</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E13" s="5" t="n">
         <v>43052</v>
@@ -3379,24 +3358,24 @@
         <v>2017</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>43052</v>
@@ -3414,24 +3393,24 @@
         <v>2017</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>43052</v>
@@ -3449,15 +3428,15 @@
         <v>2017</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>128</v>
@@ -3466,7 +3445,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>43052</v>
@@ -3484,24 +3463,24 @@
         <v>2017</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>43052</v>
@@ -3519,24 +3498,24 @@
         <v>2017</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>43052</v>
@@ -3554,24 +3533,24 @@
         <v>2017</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>43052</v>
@@ -3589,24 +3568,24 @@
         <v>2017</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>43052</v>
@@ -3624,24 +3603,24 @@
         <v>2017</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>43052</v>
@@ -3659,24 +3638,24 @@
         <v>2017</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>43086</v>
@@ -3694,10 +3673,10 @@
         <v>2017</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -3705,13 +3684,13 @@
         <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>43112</v>
@@ -3729,10 +3708,10 @@
         <v>2018</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -3746,7 +3725,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>43052</v>
@@ -3764,10 +3743,10 @@
         <v>2017</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -3781,7 +3760,7 @@
         <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>43146</v>
@@ -3799,10 +3778,10 @@
         <v>2018</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -3810,13 +3789,13 @@
         <v>2</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>43165</v>
@@ -3834,24 +3813,24 @@
         <v>2018</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E27" s="5" t="n">
         <v>43165</v>
@@ -3869,10 +3848,10 @@
         <v>2018</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -3886,7 +3865,7 @@
         <v>1</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E28" s="5" t="n">
         <v>43052</v>
@@ -3904,10 +3883,10 @@
         <v>2017</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -3921,7 +3900,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="E29" s="5" t="n">
         <v>43052</v>
@@ -3936,10 +3915,10 @@
         <v>2018</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -3953,13 +3932,13 @@
         <v>29</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="E30" s="5" t="n">
         <v>43052</v>
       </c>
       <c r="F30" s="1" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G30" s="1" t="n">
         <v>10</v>
@@ -3968,10 +3947,10 @@
         <v>2018</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -3985,13 +3964,13 @@
         <v>29</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="E31" s="5" t="n">
         <v>43052</v>
       </c>
       <c r="F31" s="1" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G31" s="1" t="n">
         <v>10</v>
@@ -4000,10 +3979,10 @@
         <v>2018</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -4017,13 +3996,13 @@
         <v>29</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="E32" s="5" t="n">
         <v>43052</v>
       </c>
       <c r="F32" s="1" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G32" s="1" t="n">
         <v>10</v>
@@ -4032,10 +4011,10 @@
         <v>2018</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -4049,13 +4028,13 @@
         <v>29</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="E33" s="5" t="n">
         <v>43052</v>
       </c>
       <c r="F33" s="1" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G33" s="1" t="n">
         <v>10</v>
@@ -4064,10 +4043,10 @@
         <v>2018</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -4081,13 +4060,13 @@
         <v>29</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="E34" s="5" t="n">
         <v>43052</v>
       </c>
       <c r="F34" s="1" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G34" s="1" t="n">
         <v>10</v>
@@ -4096,10 +4075,10 @@
         <v>2018</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -4113,13 +4092,13 @@
         <v>29</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>43052</v>
       </c>
       <c r="F35" s="1" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G35" s="1" t="n">
         <v>10</v>
@@ -4128,10 +4107,10 @@
         <v>2018</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -4145,13 +4124,13 @@
         <v>29</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>43052</v>
       </c>
       <c r="F36" s="1" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G36" s="1" t="n">
         <v>10</v>
@@ -4160,10 +4139,10 @@
         <v>2018</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -4177,13 +4156,13 @@
         <v>29</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="E37" s="5" t="n">
         <v>43052</v>
       </c>
       <c r="F37" s="1" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G37" s="1" t="n">
         <v>10</v>
@@ -4192,10 +4171,10 @@
         <v>2018</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -4209,7 +4188,7 @@
         <v>1</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>43278</v>
@@ -4224,10 +4203,10 @@
         <v>2018</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -4241,7 +4220,7 @@
         <v>1</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>43278</v>
@@ -4256,17 +4235,49 @@
         <v>2018</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E40" s="5" t="n">
+        <v>43397</v>
+      </c>
+      <c r="F40" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="G40" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="H40" s="1" t="n">
+        <v>2018</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1540016988" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1540462101" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -4275,14 +4286,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1540016988" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1540016988" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1540462101" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1540462101" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1540016988" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1540462101" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -4293,10 +4304,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView view="normal" zoomScale="110" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
@@ -4305,353 +4316,287 @@
     <col min="2" max="2" width="16.714286" customWidth="1"/>
     <col min="3" max="3" width="63.982143" customWidth="1"/>
     <col min="4" max="4" width="19.714286" customWidth="1"/>
-    <col min="5" max="5" width="14.142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2"/>
       <c r="C2" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D2" t="s">
-        <v>245</v>
-      </c>
-      <c r="E2" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
+      <c r="B3"/>
       <c r="C3" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D3" t="s">
-        <v>245</v>
-      </c>
-      <c r="E3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>6</v>
       </c>
+      <c r="B4"/>
       <c r="C4" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D4" t="s">
-        <v>245</v>
-      </c>
-      <c r="E4" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>8</v>
       </c>
+      <c r="B5"/>
       <c r="C5" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D5" t="s">
-        <v>245</v>
-      </c>
-      <c r="E5" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>10</v>
       </c>
+      <c r="B6"/>
       <c r="C6" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D6" t="s">
-        <v>245</v>
-      </c>
-      <c r="E6" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>12</v>
       </c>
+      <c r="B7"/>
       <c r="C7" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D7" t="s">
-        <v>245</v>
-      </c>
-      <c r="E7" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>14</v>
       </c>
+      <c r="B8"/>
       <c r="C8" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D8" t="s">
-        <v>248</v>
-      </c>
-      <c r="E8" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>250</v>
       </c>
       <c r="D9" t="s">
         <v>251</v>
       </c>
-      <c r="E9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
         <v>252</v>
       </c>
-      <c r="D10" t="s">
-        <v>253</v>
-      </c>
-      <c r="E10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>16</v>
       </c>
       <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
         <v>254</v>
       </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
         <v>255</v>
       </c>
-      <c r="E11" t="s">
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>125</v>
+      </c>
+      <c r="B14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
+      <c r="D14" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="s">
-        <v>256</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="D15" t="s">
         <v>257</v>
       </c>
-      <c r="E12" t="s">
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
+      <c r="D16" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" t="s">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
-        <v>258</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="D17" t="s">
         <v>259</v>
       </c>
-      <c r="E13" t="s">
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
+      <c r="D18" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s">
-        <v>260</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="D19" t="s">
         <v>261</v>
       </c>
-      <c r="E14" t="s">
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
+      <c r="D20" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21" t="s">
         <v>16</v>
       </c>
-      <c r="B15" t="s">
-        <v>262</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="D21" t="s">
         <v>263</v>
       </c>
-      <c r="E15" t="s">
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
+      <c r="D22" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" t="s">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
-        <v>264</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="D23" t="s">
         <v>265</v>
       </c>
-      <c r="E16" t="s">
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>125</v>
+      </c>
+      <c r="B24" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="D24" t="s">
         <v>266</v>
-      </c>
-      <c r="D17" t="s">
-        <v>267</v>
-      </c>
-      <c r="E17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>268</v>
-      </c>
-      <c r="D18" t="s">
-        <v>269</v>
-      </c>
-      <c r="E18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" t="s">
-        <v>270</v>
-      </c>
-      <c r="D19" t="s">
-        <v>271</v>
-      </c>
-      <c r="E19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" t="s">
-        <v>272</v>
-      </c>
-      <c r="D20" t="s">
-        <v>273</v>
-      </c>
-      <c r="E20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" t="s">
-        <v>274</v>
-      </c>
-      <c r="D21" t="s">
-        <v>275</v>
-      </c>
-      <c r="E21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" t="s">
-        <v>276</v>
-      </c>
-      <c r="D22" t="s">
-        <v>277</v>
-      </c>
-      <c r="E22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" t="s">
-        <v>278</v>
-      </c>
-      <c r="D23" t="s">
-        <v>279</v>
-      </c>
-      <c r="E23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" t="s">
-        <v>280</v>
-      </c>
-      <c r="D24" t="s">
-        <v>281</v>
-      </c>
-      <c r="E24" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1540016988" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1540462101" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -4660,14 +4605,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1540016988" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1540016988" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1540462101" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1540462101" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1540016988" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1540462101" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -4678,56 +4623,60 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView view="normal" zoomScale="120" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="15.40"/>
   <cols>
     <col min="1" max="1" width="11.455357" customWidth="1"/>
-    <col min="2" max="2" width="16.714286" customWidth="1"/>
+    <col min="2" max="2" width="18.125000" customWidth="1"/>
     <col min="3" max="3" width="11.571429" customWidth="1"/>
     <col min="4" max="4" width="19.142857" customWidth="1"/>
-    <col min="5" max="5" width="11.571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:3">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>269</v>
+      </c>
+      <c r="D2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C3" t="s">
-        <v>284</v>
+        <v>271</v>
+      </c>
+      <c r="D3" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4735,13 +4684,13 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C4" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
       <c r="D4" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4749,53 +4698,20 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C5" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
       <c r="D5" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>258</v>
-      </c>
-      <c r="C6" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>260</v>
-      </c>
-      <c r="C7" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>264</v>
-      </c>
-      <c r="C8" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1540016988" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1540462101" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -4804,14 +4720,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1540016988" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1540016988" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1540462101" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1540462101" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1540016988" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1540462101" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -4822,10 +4738,97 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView view="normal" zoomScale="120" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="15.40"/>
+  <cols>
+    <col min="1" max="1" width="11.455357" customWidth="1"/>
+    <col min="2" max="2" width="15.080357" customWidth="1"/>
+    <col min="3" max="3" width="11.562500" customWidth="1"/>
+    <col min="4" max="4" width="19.142857" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1540462101" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="1.000000" right="1.000000" top="1.000000" bottom="1.000000" header="0.393750" footer="0.393750"/>
+  <pageSetup paperSize="1" fitToWidth="0" fitToHeight="1" pageOrder="overThenDown"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1540462101" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1540462101" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+      </ext>
+    </extLst>
+  </headerFooter>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1540462101" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
@@ -4842,16 +4845,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4859,7 +4862,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -4870,21 +4873,24 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -4892,7 +4898,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -4903,7 +4909,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -4914,7 +4920,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -4925,13 +4931,13 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="C8" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="D8" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4939,13 +4945,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="C9" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="D9" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -4953,13 +4959,13 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="C10" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="D10" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -4967,13 +4973,13 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="C11" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="D11" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -4981,13 +4987,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="C12" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
       <c r="D12" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -4995,13 +5001,13 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="C13" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="D13" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -5009,13 +5015,13 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="C14" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="D14" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -5023,13 +5029,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="C15" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="D15" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -5037,13 +5043,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="C16" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="D16" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -5051,13 +5057,13 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="C17" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="D17" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -5065,7 +5071,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -5075,7 +5081,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1540016988" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1540462101" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -5084,14 +5090,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1540016988" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1540016988" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1540462101" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1540462101" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1540016988" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1540462101" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -5100,7 +5106,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -5122,16 +5128,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5139,10 +5145,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="D2" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5150,10 +5156,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="D3" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -5161,14 +5167,14 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="C4" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>317</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5176,13 +5182,13 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="D5" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="E5" t="s">
-        <v>317</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -5190,20 +5196,20 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="D6" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="E6" t="s">
-        <v>317</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1540016988" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1540462101" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -5212,14 +5218,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1540016988" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1540016988" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1540462101" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1540462101" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1540016988" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1540462101" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>